<commit_message>
Made sure to accomondate for converting from deg per second to rad per second. I have now pulled from the correct column to match with the data that is pulled from Pradeeps Excel. Lastly, I have made sure to adjust the angle obtained from 360 to 180 degrees from within WitMotion.
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results\E\AngVel\f10RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B61D02-91EA-46FF-ACE1-A35B58224823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02BE48C-8CE7-471A-8C10-63174AA7275C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="240" windowWidth="15120" windowHeight="8604" xr2:uid="{3B02BD5D-EA7C-4DC7-9543-9456AFADE48E}"/>
+    <workbookView xWindow="5040" yWindow="240" windowWidth="15120" windowHeight="8604" xr2:uid="{1837FA33-78D6-45B3-89D3-0B34CB12EA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB253950-9573-4815-A274-077FE4A307AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BC1335-D888-469F-97B2-265476EF066F}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
starter code before accounting for decimal place for input speed
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results\E\AngVel\f10RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02BE48C-8CE7-471A-8C10-63174AA7275C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E520B5-DA11-4CA7-8250-E23AE314810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="240" windowWidth="15120" windowHeight="8604" xr2:uid="{1837FA33-78D6-45B3-89D3-0B34CB12EA7F}"/>
+    <workbookView xWindow="348" yWindow="1092" windowWidth="15120" windowHeight="10788" xr2:uid="{5CA40D7A-8BD0-4BEF-B665-6C8179F2FBFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BC1335-D888-469F-97B2-265476EF066F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0756DC-6940-4855-94B7-7E247F9D8362}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0.64598979481797014</v>
+        <v>6.4936089473162595E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>